<commit_message>
mp5 weight increase + stocks swap
</commit_message>
<xml_diff>
--- a/changes/mp5.xlsx
+++ b/changes/mp5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifan/Documents/deadline-balancing/changes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA48152-32F1-43AE-9072-3F7E55364DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BC23CF-4C1A-C743-A6B7-E526A41ED9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>new</t>
   </si>
@@ -80,36 +80,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>hk_mp5_wide_tropical_handguard</t>
-  </si>
-  <si>
-    <t>HK MP5 Wide Tropical</t>
-  </si>
-  <si>
-    <t>hk_mp5sd_polymer_handguard</t>
-  </si>
-  <si>
-    <t>HK MP5SD Polymer Handguard</t>
-  </si>
-  <si>
-    <t>hk_mp5_slim_checkered_handguard</t>
-  </si>
-  <si>
-    <t>HK MP5 Slim Checkered Handguard</t>
-  </si>
-  <si>
-    <t>midwest_industries_mp5_mlok_handguard</t>
-  </si>
-  <si>
-    <t>Midwest Industries MP5 MLOK Handguard</t>
-  </si>
-  <si>
-    <t>surefire_628lmf_b_mp5_handguard</t>
-  </si>
-  <si>
-    <t>Surefire 628LMF-B MP5 Handguard</t>
-  </si>
-  <si>
     <t>hk_mp5a3_early_gen_stock_endplate</t>
   </si>
   <si>
@@ -131,25 +101,31 @@
     <t>hk_mp5_hk94_stock_endcap</t>
   </si>
   <si>
-    <t>HP MP5/HK94 Stock Endcap</t>
-  </si>
-  <si>
     <t>hk_mp5_endcap_sling_swivel</t>
   </si>
   <si>
     <t>HK MP5 Endcap Sling Swivel</t>
   </si>
   <si>
-    <t>hk_mp5_hk94_choate_stock_base</t>
-  </si>
-  <si>
-    <t>HK MP5/HK94 Choate Stock Base</t>
-  </si>
-  <si>
-    <t>hk_mp5_hk94_choate_stock</t>
-  </si>
-  <si>
-    <t>HK MP5/HK94 Choate Stock</t>
+    <t>hk_mp5_hk94_cartman_stock_base</t>
+  </si>
+  <si>
+    <t>hk_mp5_hk94_cartman_stock</t>
+  </si>
+  <si>
+    <t>HK MP5/HK94 Cartman Stock Base</t>
+  </si>
+  <si>
+    <t>HK MP5/HK94 Cartman Stock</t>
+  </si>
+  <si>
+    <t>mp5a3</t>
+  </si>
+  <si>
+    <t>cartman</t>
+  </si>
+  <si>
+    <t>HK MP5/HK94 Stock Endcap</t>
   </si>
 </sst>
 </file>
@@ -633,9 +609,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -695,9 +670,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -735,7 +710,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -841,7 +816,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -983,7 +958,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -991,628 +966,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="22" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" customWidth="1"/>
+    <col min="3" max="22" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0.25</v>
+      </c>
+      <c r="E3">
+        <v>-10</v>
+      </c>
+      <c r="F3">
+        <v>-12</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
+        <v>18.2</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="M4">
+        <v>1500</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
         <v>-9</v>
       </c>
-      <c r="F5" s="1">
-        <v>-7</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" ref="N5:N17" si="0">C5-D5*20-E5*0.8-F5*0.6-H5*5+I5*10+J5/300</f>
-        <v>15.8</v>
+      <c r="F5">
+        <v>-9</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>20.599999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-6</v>
-      </c>
-      <c r="F6" s="1">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M6">
+        <v>1000</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>-1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.05</v>
+      </c>
+      <c r="M7">
+        <v>750</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>0.12</v>
+      </c>
+      <c r="E8">
         <v>-8</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1">
-        <v>2000</v>
-      </c>
-      <c r="N6" s="1">
+      <c r="F8">
+        <v>-13</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="0"/>
-        <v>16.2</v>
+        <v>20.8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>0.01</v>
+      </c>
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>-6</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0.2</v>
+      </c>
+      <c r="M9">
+        <v>250</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>-3.1999999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <f>C4+C5</f>
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <f>D4+D5</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:M11" si="1">E4+E5</f>
+        <v>-9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
         <v>1500</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N11">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>18.599999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-9</v>
-      </c>
-      <c r="F8" s="1">
-        <v>-9</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1">
-        <v>1200</v>
-      </c>
-      <c r="N8" s="1">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <f>C6+C7+C8</f>
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:M12" si="2">D6+D7+D8</f>
+        <v>0.24</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>-13</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>1750</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="0"/>
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-6</v>
-      </c>
-      <c r="F9" s="1">
-        <v>-7</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-10</v>
-      </c>
-      <c r="F11" s="1">
-        <v>-12</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>0.08</v>
-      </c>
-      <c r="M12">
-        <v>1500</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.39999999999999991</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>0.12</v>
-      </c>
-      <c r="E13">
-        <v>-9</v>
-      </c>
-      <c r="F13">
-        <v>-8</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="0"/>
-        <v>18.600000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>0.06</v>
-      </c>
-      <c r="M14">
-        <v>1000</v>
-      </c>
-      <c r="N14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1">
-        <v>750</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E16" s="1">
-        <v>-8</v>
-      </c>
-      <c r="F16" s="1">
-        <v>-13</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="0"/>
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E17" s="1">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1">
-        <v>10</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1">
-        <v>250</v>
-      </c>
-      <c r="N17" s="1">
-        <f t="shared" si="0"/>
-        <v>-5.1999999999999993</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N40" s="1"/>
+        <v>18.400000000000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>